<commit_message>
todas las funciones fitness
</commit_message>
<xml_diff>
--- a/Plantilla_Horario.xlsx
+++ b/Plantilla_Horario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DALIA\Schedule-Generator-AG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\Proyecto Seminario de Algoritmia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B11B7600-C21F-4D09-9386-E7ABCA1C1257}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1FC9DD-F64A-4815-8E4C-7A49E8F09FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F56D63F2-97B0-4BD1-B0C9-D23A4D4A050D}"/>
+    <workbookView xWindow="8280" yWindow="1365" windowWidth="17700" windowHeight="11385" xr2:uid="{F56D63F2-97B0-4BD1-B0C9-D23A4D4A050D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
   <si>
     <t>Materia</t>
   </si>
@@ -597,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF99C014-A569-482F-9854-47235F4B3C3F}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,79 +649,79 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E4">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
         <v>5</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="E6">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -729,82 +729,82 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="E7">
         <v>10</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F8">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
         <v>35</v>
       </c>
       <c r="E9">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F9">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E10">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F10">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -829,19 +829,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E12">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F12">
         <v>3</v>
@@ -849,159 +849,159 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13">
         <v>6</v>
       </c>
-      <c r="C13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13">
-        <v>10</v>
-      </c>
       <c r="F13">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="E14">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F14">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E15">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F16">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E17">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F17">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="E18">
+        <v>7</v>
+      </c>
+      <c r="F18">
         <v>5</v>
-      </c>
-      <c r="F18">
-        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="E19">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F19">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="E20">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F20">
         <v>2</v>
@@ -1009,139 +1009,139 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="E21">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F21">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E22">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
+        <v>17</v>
       </c>
       <c r="E23">
+        <v>9</v>
+      </c>
+      <c r="F23">
         <v>5</v>
-      </c>
-      <c r="F23">
-        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="E24">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E25">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="E26">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F26">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D27" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E27">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F27">
         <v>4</v>
@@ -1149,22 +1149,22 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D28" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E28">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1172,39 +1172,45 @@
         <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D29" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="E29">
         <v>4</v>
       </c>
       <c r="F29">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="D30" t="s">
+        <v>68</v>
       </c>
       <c r="E30">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F30">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F30">
+    <sortCondition ref="A2:A30"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
implementacion de excel para resultados
</commit_message>
<xml_diff>
--- a/Plantilla_Horario.xlsx
+++ b/Plantilla_Horario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\Proyecto Seminario de Algoritmia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFA42C2-557B-49C3-955E-E54A4CD121D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E11B71-BB3F-4BFA-823C-CB48F4052938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4830" yWindow="2610" windowWidth="17700" windowHeight="11385" xr2:uid="{F56D63F2-97B0-4BD1-B0C9-D23A4D4A050D}"/>
   </bookViews>
@@ -616,7 +616,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>